<commit_message>
Xiang guo pilot 3
</commit_message>
<xml_diff>
--- a/FilmFinder/FilmFinder/bin/Debug/Pilots and trials/Subject 6 - third pilot by paymahn.xlsx
+++ b/FilmFinder/FilmFinder/bin/Debug/Pilots and trials/Subject 6 - third pilot by paymahn.xlsx
@@ -717,11 +717,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="107095552"/>
-        <c:axId val="107097088"/>
+        <c:axId val="96597888"/>
+        <c:axId val="96599424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107095552"/>
+        <c:axId val="96597888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +730,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107097088"/>
+        <c:crossAx val="96599424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -738,7 +738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107097088"/>
+        <c:axId val="96599424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,7 +749,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107095552"/>
+        <c:crossAx val="96597888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1113,11 +1113,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="107128320"/>
-        <c:axId val="107129856"/>
+        <c:axId val="99067776"/>
+        <c:axId val="99069312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107128320"/>
+        <c:axId val="99067776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1126,7 +1126,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107129856"/>
+        <c:crossAx val="99069312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1134,7 +1134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107129856"/>
+        <c:axId val="99069312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,7 +1145,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107128320"/>
+        <c:crossAx val="99067776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1509,11 +1509,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="118842880"/>
-        <c:axId val="118844416"/>
+        <c:axId val="100947840"/>
+        <c:axId val="100949376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118842880"/>
+        <c:axId val="100947840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1522,7 +1522,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118844416"/>
+        <c:crossAx val="100949376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1530,7 +1530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118844416"/>
+        <c:axId val="100949376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1541,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118842880"/>
+        <c:crossAx val="100947840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1567,16 +1567,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1598,15 +1598,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1628,15 +1628,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1948,8 +1948,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>